<commit_message>
Update before extraction of echolocatoR to separate repo
</commit_message>
<xml_diff>
--- a/echolocatoR/annotations/Nott_2019/Nott_2019.snEpigenomics.xlsx
+++ b/echolocatoR/annotations/Nott_2019/Nott_2019.snEpigenomics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Fine_Mapping/echolocatoR/annotations/Glass_lab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Fine_Mapping/echolocatoR/annotations/Nott_2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B8E3D7-A111-4C48-ADDD-6FAA7A43B8B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6265D093-3562-2E48-9C74-F121077EF003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="460" windowWidth="38220" windowHeight="18340" xr2:uid="{010F0F86-E4AD-7D4F-87C8-55A1C5C6F5BF}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{010F0F86-E4AD-7D4F-87C8-55A1C5C6F5BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="67">
   <si>
     <t> schema </t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>peripheral PU1+</t>
+  </si>
+  <si>
+    <t>minerva_link</t>
   </si>
 </sst>
 </file>
@@ -621,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F20365B-2B7B-E647-B034-C96F4CC885A9}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -639,7 +642,7 @@
     <col min="11" max="11" width="108.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -673,8 +676,11 @@
       <c r="K1" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L1" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -710,8 +716,12 @@
         <f>I2&amp;J2&amp;"/"&amp;B2&amp;".ucsc.bigWig"</f>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k27ac_hg19_pooled/hg19/human_microglia_H3K27ac_exvivo_pooled_hg19.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L2" s="4" t="str">
+        <f>_xlfn.CONCAT("/pd-omics/data/Nott_2019/",B2,".ucsc.bigWig")</f>
+        <v>/pd-omics/data/Nott_2019/human_microglia_H3K27ac_exvivo_pooled_hg19.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -747,8 +757,12 @@
         <f t="shared" ref="K3:K19" si="1">I3&amp;J3&amp;"/"&amp;B3&amp;".ucsc.bigWig"</f>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k27ac_hg19_pooled/hg19/human_microglia_H3K27ac_exvivo_pooled_hg19_tbp.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L3" s="4" t="str">
+        <f t="shared" ref="L3:L19" si="2">_xlfn.CONCAT("/pd-omics/data/Nott_2019/",B3,".ucsc.bigWig")</f>
+        <v>/pd-omics/data/Nott_2019/human_microglia_H3K27ac_exvivo_pooled_hg19_tbp.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -784,8 +798,12 @@
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k27ac_hg19_pooled/hg19/human_PU1nuclei_H3K27ac_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>/pd-omics/data/Nott_2019/human_PU1nuclei_H3K27ac_epilepsy_pooled_hg19.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -821,8 +839,12 @@
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k27ac_hg19_pooled/hg19/human_NEUNnuclei_H3K27ac_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>/pd-omics/data/Nott_2019/human_NEUNnuclei_H3K27ac_epilepsy_pooled_hg19.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -858,8 +880,12 @@
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k27ac_hg19_pooled/hg19/human_OLIG2nuclei_H3K27ac_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>/pd-omics/data/Nott_2019/human_OLIG2nuclei_H3K27ac_epilepsy_pooled_hg19.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -895,8 +921,12 @@
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k27ac_hg19_pooled/hg19/human_peripheralPU1nuclei_H3K27ac_hg19.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>/pd-omics/data/Nott_2019/human_peripheralPU1nuclei_H3K27ac_hg19.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -932,8 +962,12 @@
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k27ac_hg19_pooled/hg19/human_LHX2nuclei_H3K27ac_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>/pd-omics/data/Nott_2019/human_LHX2nuclei_H3K27ac_epilepsy_pooled_hg19.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -969,8 +1003,12 @@
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_atac_hg19_pooled/hg19/human_microglia_atac_exvivo_pooled_hg19.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>/pd-omics/data/Nott_2019/human_microglia_atac_exvivo_pooled_hg19.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1006,8 +1044,12 @@
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_atac_hg19_pooled/hg19/human_microglia_atac_exvivo_pooled_hg19_tbp.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>/pd-omics/data/Nott_2019/human_microglia_atac_exvivo_pooled_hg19_tbp.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -1043,8 +1085,12 @@
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_atac_hg19_pooled/hg19/human_PU1nuclei_atac_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>/pd-omics/data/Nott_2019/human_PU1nuclei_atac_epilepsy_pooled_hg19.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -1080,8 +1126,12 @@
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_atac_hg19_pooled/hg19/human_NEUNnuclei_atac_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>/pd-omics/data/Nott_2019/human_NEUNnuclei_atac_epilepsy_pooled_hg19.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -1117,8 +1167,12 @@
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_atac_hg19_pooled/hg19/human_OLIG2nuclei_atac_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>/pd-omics/data/Nott_2019/human_OLIG2nuclei_atac_epilepsy_pooled_hg19.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -1154,8 +1208,12 @@
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_atac_hg19_pooled/hg19/human_peripheralPU1nuclei_atac_hg19.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>/pd-omics/data/Nott_2019/human_peripheralPU1nuclei_atac_hg19.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -1191,8 +1249,12 @@
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_atac_hg19_pooled/hg19/human_LHX2nuclei_atac_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>/pd-omics/data/Nott_2019/human_LHX2nuclei_atac_epilepsy_pooled_hg19.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
@@ -1228,8 +1290,12 @@
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k4me3_hg19_pooled/hg19/human_PU1nuclei_H3K4me3_epilepsy_hg19.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>/pd-omics/data/Nott_2019/human_PU1nuclei_H3K4me3_epilepsy_hg19.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -1265,8 +1331,12 @@
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k4me3_hg19_pooled/hg19/human_NEUNnuclei_H3K4me3_epilepsy_hg19.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>/pd-omics/data/Nott_2019/human_NEUNnuclei_H3K4me3_epilepsy_hg19.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
@@ -1302,8 +1372,12 @@
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k4me3_hg19_pooled/hg19/human_OLIG2nuclei_H3K4me3_epilepsy_hg19.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>/pd-omics/data/Nott_2019/human_OLIG2nuclei_H3K4me3_epilepsy_hg19.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
@@ -1339,8 +1413,12 @@
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k4me3_hg19_pooled/hg19/human_LHX2nuclei_H3K4me3_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>/pd-omics/data/Nott_2019/human_LHX2nuclei_H3K4me3_epilepsy_pooled_hg19.ucsc.bigWig</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
     </row>

</xml_diff>